<commit_message>
Site updated: 2024-05-15 17:46:04
</commit_message>
<xml_diff>
--- a/pdf/血常规曲线图.xlsx
+++ b/pdf/血常规曲线图.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\websrv\blog\source\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C03D69-3C6F-4983-82D0-0FFE53B90A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDF03A1-FD1E-4E88-A40D-94EE078BC7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,15 +107,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -123,20 +129,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3128,7 +3151,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3141,7 +3164,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="2"/>
@@ -3152,222 +3175,226 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="A3" s="4">
         <v>45335</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>3.11</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>2.3170000000000002</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>77</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="5">
         <v>95</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+      <c r="A4" s="4">
         <v>45337</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>1.55</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>0.98899999999999999</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>1.72</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="5">
         <v>64</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="5">
         <v>84</v>
       </c>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="4">
         <v>45342</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>1.1399999999999999</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>0.53200000000000003</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>1.76</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>64</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>121</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="A6" s="4">
         <v>45392</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>1.5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>0.71</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>1.8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="5">
         <v>70</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <v>85</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+      <c r="A7" s="4">
         <v>45395</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>1.47</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>0.65</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>1.44</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="5">
         <v>56</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="5">
         <v>71</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+      <c r="A8" s="4">
         <v>45400</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>1.42</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>0.79</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>1.36</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="5">
         <v>53</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="5">
         <v>61</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="A9" s="4">
         <v>45406</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>1.82</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>1.0900000000000001</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="5">
         <v>81</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="5">
         <v>48</v>
       </c>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
+      <c r="A10" s="4">
         <v>45413</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>1.45</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>0.63</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>71</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="5">
         <v>69</v>
       </c>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
+      <c r="A11" s="4">
         <v>45427</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>1.44</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>0.53</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <v>1.84</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>68</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <v>79</v>
       </c>
+      <c r="G11" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Site updated: 2024-05-16 15:48:37
</commit_message>
<xml_diff>
--- a/pdf/血常规曲线图.xlsx
+++ b/pdf/血常规曲线图.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\websrv\blog\source\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDF03A1-FD1E-4E88-A40D-94EE078BC7D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B192FA30-20E2-40D8-9051-A272BC10AB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -151,15 +151,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -976,10 +976,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="105"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="5"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -1062,7 +1062,9 @@
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3">
+                  <a:shade val="76000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1073,7 +1075,9 @@
             <c:size val="17"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3">
+                  <a:shade val="76000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1231,7 +1235,9 @@
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent3">
+                  <a:tint val="77000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1242,7 +1248,9 @@
             <c:size val="17"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent3">
+                  <a:tint val="77000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1633,42 +1641,8 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="16">
   <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
 </cs:colorStyle>
 </file>
 
@@ -2888,7 +2862,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="自定义 1">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2902,16 +2876,16 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="BDD7EE"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="FF0000"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="7030A0"/>
       </a:accent4>
       <a:accent5>
         <a:srgbClr val="4472C4"/>
@@ -3151,7 +3125,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3164,237 +3138,237 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>45335</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>3.11</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>2.3170000000000002</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>77</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>95</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>45337</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>1.55</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>0.98899999999999999</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>1.72</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>64</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>84</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>45342</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>1.1399999999999999</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>0.53200000000000003</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>1.76</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>64</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>121</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>45392</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>1.5</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>0.71</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>1.8</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>70</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>85</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>45395</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>1.47</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>0.65</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>1.44</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>56</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>71</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>45400</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>1.42</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>0.79</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>1.36</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>53</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>61</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>45406</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="3">
         <v>1.82</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>1.0900000000000001</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>81</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>48</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <v>45413</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="3">
         <v>1.45</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>0.63</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>2</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>71</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>69</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <v>45427</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="3">
         <v>1.44</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>0.53</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>1.84</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>68</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>79</v>
       </c>
-      <c r="G11" s="5"/>
+      <c r="G11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Site updated: 2024-05-16 16:35:27
</commit_message>
<xml_diff>
--- a/pdf/血常规曲线图.xlsx
+++ b/pdf/血常规曲线图.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\websrv\blog\source\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B192FA30-20E2-40D8-9051-A272BC10AB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A1810E-813A-4DDA-9FC2-0E53D44DCEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1005" yWindow="1710" windowWidth="26580" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>白细胞</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -78,6 +78,26 @@
     <t>https://qianj.itcad.club/clvp7eapn0000c0yj3vi3cg8z.html#more</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>正常最低值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>求和</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>平均值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>汇总</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -107,7 +127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +137,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,7 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -160,6 +186,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -344,72 +372,77 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>45335</c:v>
+                  <c:v>正常最低值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45337</c:v>
+                  <c:v>2024/2/13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45342</c:v>
+                  <c:v>2024/2/15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45392</c:v>
+                  <c:v>2024/2/20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45395</c:v>
+                  <c:v>2024/4/10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45400</c:v>
+                  <c:v>2024/4/13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45406</c:v>
+                  <c:v>2024/4/18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45413</c:v>
+                  <c:v>2024/4/24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45427</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>2024/5/1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2024/5/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$11</c:f>
+              <c:f>Sheet1!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>3.11</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1.55</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1.1399999999999999</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1.47</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.42</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1.82</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>1.45</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1.44</c:v>
                 </c:pt>
               </c:numCache>
@@ -513,72 +546,77 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>45335</c:v>
+                  <c:v>正常最低值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45337</c:v>
+                  <c:v>2024/2/13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45342</c:v>
+                  <c:v>2024/2/15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45392</c:v>
+                  <c:v>2024/2/20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45395</c:v>
+                  <c:v>2024/4/10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45400</c:v>
+                  <c:v>2024/4/13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45406</c:v>
+                  <c:v>2024/4/18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45413</c:v>
+                  <c:v>2024/4/24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45427</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>2024/5/1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2024/5/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$11</c:f>
+              <c:f>Sheet1!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2.3170000000000002</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>0.98899999999999999</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>0.53200000000000003</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.71</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>0.65</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>0.79</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>1.0900000000000001</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>0.63</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>0.53</c:v>
                 </c:pt>
               </c:numCache>
@@ -682,72 +720,77 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>45335</c:v>
+                  <c:v>正常最低值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45337</c:v>
+                  <c:v>2024/2/13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45342</c:v>
+                  <c:v>2024/2/15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45392</c:v>
+                  <c:v>2024/2/20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45395</c:v>
+                  <c:v>2024/4/10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45400</c:v>
+                  <c:v>2024/4/13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45406</c:v>
+                  <c:v>2024/4/18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45413</c:v>
+                  <c:v>2024/4/24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45427</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>2024/5/1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2024/5/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$11</c:f>
+              <c:f>Sheet1!$D$3:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>1.72</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>1.76</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>1.8</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>1.44</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>1.36</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>2.2000000000000002</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>1.84</c:v>
                 </c:pt>
               </c:numCache>
@@ -774,14 +817,14 @@
         <c:axId val="2087382720"/>
         <c:axId val="2087385600"/>
       </c:lineChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="2087382720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -821,9 +864,10 @@
         <c:crossAx val="2087385600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="2087385600"/>
         <c:scaling>
@@ -1140,72 +1184,77 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>45335</c:v>
+                  <c:v>正常最低值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45337</c:v>
+                  <c:v>2024/2/13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45342</c:v>
+                  <c:v>2024/2/15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45392</c:v>
+                  <c:v>2024/2/20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45395</c:v>
+                  <c:v>2024/4/10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45400</c:v>
+                  <c:v>2024/4/13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45406</c:v>
+                  <c:v>2024/4/18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45413</c:v>
+                  <c:v>2024/4/24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45427</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>2024/5/1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2024/5/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$11</c:f>
+              <c:f>Sheet1!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>70</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>81</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>71</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
@@ -1313,72 +1362,77 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$A$3:$A$11</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>45335</c:v>
+                  <c:v>正常最低值</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45337</c:v>
+                  <c:v>2024/2/13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>45342</c:v>
+                  <c:v>2024/2/15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45392</c:v>
+                  <c:v>2024/2/20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45395</c:v>
+                  <c:v>2024/4/10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45400</c:v>
+                  <c:v>2024/4/13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45406</c:v>
+                  <c:v>2024/4/18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>45413</c:v>
+                  <c:v>2024/4/24</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45427</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>2024/5/1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2024/5/15</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$11</c:f>
+              <c:f>Sheet1!$F$3:$F$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>84</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>121</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>85</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>71</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>48</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>69</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>79</c:v>
                 </c:pt>
               </c:numCache>
@@ -1387,7 +1441,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8050-4C57-A1A3-9447B4A1ABB2}"/>
+              <c16:uniqueId val="{00000000-2899-41E0-B688-094EFC650102}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1405,14 +1459,14 @@
         <c:axId val="141792880"/>
         <c:axId val="141788080"/>
       </c:lineChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="141792880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1452,9 +1506,10 @@
         <c:crossAx val="141788080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="141788080"/>
         <c:scaling>
@@ -2787,15 +2842,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
+      <xdr:colOff>4761</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>23811</xdr:rowOff>
+      <xdr:rowOff>23810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>11429</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>126142</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2823,15 +2878,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>31431</xdr:rowOff>
+      <xdr:colOff>23811</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>430209</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>59054</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3122,10 +3177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3172,203 +3227,224 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>45335</v>
-      </c>
-      <c r="B3" s="3">
-        <v>3.11</v>
-      </c>
-      <c r="C3" s="3">
-        <v>2.3170000000000002</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3">
-        <v>77</v>
-      </c>
-      <c r="F3" s="3">
-        <v>95</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1.8</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3.8</v>
+      </c>
+      <c r="E3" s="6">
+        <v>115</v>
+      </c>
+      <c r="F3" s="6">
+        <v>125</v>
+      </c>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>45337</v>
+        <v>45335</v>
       </c>
       <c r="B4" s="3">
-        <v>1.55</v>
+        <v>3.11</v>
       </c>
       <c r="C4" s="3">
-        <v>0.98899999999999999</v>
+        <v>2.3170000000000002</v>
       </c>
       <c r="D4" s="3">
-        <v>1.72</v>
+        <v>2</v>
       </c>
       <c r="E4" s="3">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="F4" s="3">
-        <v>84</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>45342</v>
+        <v>45337</v>
       </c>
       <c r="B5" s="3">
-        <v>1.1399999999999999</v>
+        <v>1.55</v>
       </c>
       <c r="C5" s="3">
-        <v>0.53200000000000003</v>
+        <v>0.98899999999999999</v>
       </c>
       <c r="D5" s="3">
-        <v>1.76</v>
+        <v>1.72</v>
       </c>
       <c r="E5" s="3">
         <v>64</v>
       </c>
       <c r="F5" s="3">
-        <v>121</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>8</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>45392</v>
+        <v>45342</v>
       </c>
       <c r="B6" s="3">
-        <v>1.5</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="C6" s="3">
-        <v>0.71</v>
+        <v>0.53200000000000003</v>
       </c>
       <c r="D6" s="3">
-        <v>1.8</v>
+        <v>1.76</v>
       </c>
       <c r="E6" s="3">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F6" s="3">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>45395</v>
+        <v>45392</v>
       </c>
       <c r="B7" s="3">
-        <v>1.47</v>
+        <v>1.5</v>
       </c>
       <c r="C7" s="3">
-        <v>0.65</v>
+        <v>0.71</v>
       </c>
       <c r="D7" s="3">
-        <v>1.44</v>
+        <v>1.8</v>
       </c>
       <c r="E7" s="3">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="F7" s="3">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>45400</v>
+        <v>45395</v>
       </c>
       <c r="B8" s="3">
-        <v>1.42</v>
+        <v>1.47</v>
       </c>
       <c r="C8" s="3">
-        <v>0.79</v>
+        <v>0.65</v>
       </c>
       <c r="D8" s="3">
-        <v>1.36</v>
+        <v>1.44</v>
       </c>
       <c r="E8" s="3">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F8" s="3">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>45406</v>
+        <v>45400</v>
       </c>
       <c r="B9" s="3">
-        <v>1.82</v>
+        <v>1.42</v>
       </c>
       <c r="C9" s="3">
-        <v>1.0900000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="D9" s="3">
-        <v>2.2000000000000002</v>
+        <v>1.36</v>
       </c>
       <c r="E9" s="3">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="F9" s="3">
-        <v>48</v>
-      </c>
-      <c r="G9" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>45413</v>
+        <v>45406</v>
       </c>
       <c r="B10" s="3">
-        <v>1.45</v>
+        <v>1.82</v>
       </c>
       <c r="C10" s="3">
-        <v>0.63</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="D10" s="3">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E10" s="3">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="F10" s="3">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
+        <v>45413</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1.45</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.63</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>71</v>
+      </c>
+      <c r="F11" s="3">
+        <v>69</v>
+      </c>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
         <v>45427</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B12" s="3">
         <v>1.44</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C12" s="3">
         <v>0.53</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D12" s="3">
         <v>1.84</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E12" s="3">
         <v>68</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F12" s="3">
         <v>79</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Site updated: 2024-05-16 17:32:06
</commit_message>
<xml_diff>
--- a/pdf/血常规曲线图.xlsx
+++ b/pdf/血常规曲线图.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\websrv\blog\source\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A1810E-813A-4DDA-9FC2-0E53D44DCEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC61E74-3D92-4211-B271-18BEF6E3883D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1005" yWindow="1710" windowWidth="26580" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3180,7 +3180,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Site updated: 2024-05-20 09:00:43
</commit_message>
<xml_diff>
--- a/pdf/血常规曲线图.xlsx
+++ b/pdf/血常规曲线图.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\websrv\blog\source\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC61E74-3D92-4211-B271-18BEF6E3883D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3A2AA9-0730-4F1B-87FD-08AAAF2F91BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1005" yWindow="1710" windowWidth="26580" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>白细胞</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,10 +71,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>无锡住院</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://qianj.itcad.club/clvp7eapn0000c0yj3vi3cg8z.html#more</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -83,19 +79,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>求和</t>
+    <t>无锡一疗住院（4.12）期间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>平均值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>汇总</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>计数</t>
+    <t>无锡二疗住院（5.18）期间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -180,14 +168,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -373,9 +361,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Sheet1!$A$3:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>正常最低值</c:v>
                 </c:pt>
@@ -405,16 +393,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2024/5/15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024/5/19</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:f>Sheet1!$B$3:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>3.5</c:v>
                 </c:pt>
@@ -444,6 +435,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.44</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -547,9 +541,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Sheet1!$A$3:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>正常最低值</c:v>
                 </c:pt>
@@ -579,16 +573,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2024/5/15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024/5/19</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$12</c:f>
+              <c:f>Sheet1!$C$3:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1.8</c:v>
                 </c:pt>
@@ -618,6 +615,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -666,64 +666,14 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="zh-CN"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
+            <c:delete val="1"/>
+            <c:extLst/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Sheet1!$A$3:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>正常最低值</c:v>
                 </c:pt>
@@ -753,16 +703,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2024/5/15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024/5/19</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$12</c:f>
+              <c:f>Sheet1!$D$3:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>3.8</c:v>
                 </c:pt>
@@ -792,6 +745,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.84</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1185,9 +1141,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Sheet1!$A$3:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>正常最低值</c:v>
                 </c:pt>
@@ -1217,16 +1173,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2024/5/15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024/5/19</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$12</c:f>
+              <c:f>Sheet1!$E$3:$E$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>115</c:v>
                 </c:pt>
@@ -1256,6 +1215,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,9 +1325,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Sheet1!$A$3:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>正常最低值</c:v>
                 </c:pt>
@@ -1395,16 +1357,19 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2024/5/15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2024/5/19</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$12</c:f>
+              <c:f>Sheet1!$F$3:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>125</c:v>
                 </c:pt>
@@ -1434,6 +1399,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1441,7 +1409,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-2899-41E0-B688-094EFC650102}"/>
+              <c16:uniqueId val="{00000000-BDBA-4751-BE1B-841586459CBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3177,7 +3145,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
@@ -3189,19 +3157,19 @@
     <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="A1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -3227,25 +3195,25 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4">
         <v>3.5</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="4">
         <v>1.8</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="4">
         <v>3.8</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="4">
         <v>115</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="4">
         <v>125</v>
       </c>
-      <c r="G3" s="6"/>
+      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -3357,7 +3325,7 @@
         <v>71</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3445,6 +3413,29 @@
         <v>79</v>
       </c>
       <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>45431</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1.29</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.65</v>
+      </c>
+      <c r="E13" s="3">
+        <v>60</v>
+      </c>
+      <c r="F13" s="3">
+        <v>58</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Site updated: 2024-05-28 10:03:41
</commit_message>
<xml_diff>
--- a/pdf/血常规曲线图.xlsx
+++ b/pdf/血常规曲线图.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\websrv\blog\source\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD3A2AA9-0730-4F1B-87FD-08AAAF2F91BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FB8DF0-3050-4186-AF8D-A56BE8FD6613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>白细胞</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,10 +67,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>无锡出院前一天</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>https://qianj.itcad.club/clvp7eapn0000c0yj3vi3cg8z.html#more</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -84,6 +80,14 @@
   </si>
   <si>
     <t>无锡二疗住院（5.18）期间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无锡一疗出院前一天</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无锡二疗出院前一天</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -163,7 +167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -176,6 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -667,7 +672,6 @@
           </c:marker>
           <c:dLbls>
             <c:delete val="1"/>
-            <c:extLst/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -3145,10 +3149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3162,7 +3166,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -3196,7 +3200,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4">
         <v>3.5</v>
@@ -3325,7 +3329,7 @@
         <v>71</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -3348,7 +3352,7 @@
         <v>61</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -3434,7 +3438,30 @@
         <v>58</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>45436</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.82</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1.87</v>
+      </c>
+      <c r="E14" s="3">
+        <v>67</v>
+      </c>
+      <c r="F14" s="3">
+        <v>62</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Site updated: 2024-06-07 09:03:04
</commit_message>
<xml_diff>
--- a/pdf/血常规曲线图.xlsx
+++ b/pdf/血常规曲线图.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\websrv\blog\source\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FB8DF0-3050-4186-AF8D-A56BE8FD6613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DEE203-191B-467B-A9B5-91097B9A5179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>白细胞</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,15 +79,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>无锡二疗住院（5.18）期间</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>无锡一疗出院前一天</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>无锡二疗出院前一天</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>异常细胞形态：红细胞：大小不均</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无锡二疗住院（5.18）期间。异常细胞形态：红细胞：大小不均</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>异常细胞形态：红细胞：体积偏大</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -167,20 +175,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -366,9 +377,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$13</c:f>
+              <c:f>Sheet1!$A$3:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>正常最低值</c:v>
                 </c:pt>
@@ -401,16 +412,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2024/5/19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024/5/24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2024/6/5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$13</c:f>
+              <c:f>Sheet1!$B$3:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>3.5</c:v>
                 </c:pt>
@@ -443,6 +460,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -546,9 +569,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$13</c:f>
+              <c:f>Sheet1!$A$3:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>正常最低值</c:v>
                 </c:pt>
@@ -581,16 +604,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2024/5/19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024/5/24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2024/6/5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$13</c:f>
+              <c:f>Sheet1!$C$3:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>1.8</c:v>
                 </c:pt>
@@ -623,6 +652,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.63</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -675,9 +710,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$13</c:f>
+              <c:f>Sheet1!$A$3:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>正常最低值</c:v>
                 </c:pt>
@@ -710,16 +745,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2024/5/19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024/5/24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2024/6/5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$13</c:f>
+              <c:f>Sheet1!$D$3:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>3.8</c:v>
                 </c:pt>
@@ -752,6 +793,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.87</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1145,9 +1192,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$13</c:f>
+              <c:f>Sheet1!$A$3:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>正常最低值</c:v>
                 </c:pt>
@@ -1180,16 +1227,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2024/5/19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024/5/24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2024/6/5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$13</c:f>
+              <c:f>Sheet1!$E$3:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>115</c:v>
                 </c:pt>
@@ -1222,6 +1275,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1329,9 +1388,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$13</c:f>
+              <c:f>Sheet1!$A$3:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>正常最低值</c:v>
                 </c:pt>
@@ -1364,16 +1423,22 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2024/5/19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2024/5/24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2024/6/5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$13</c:f>
+              <c:f>Sheet1!$F$3:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>125</c:v>
                 </c:pt>
@@ -1406,6 +1471,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3149,19 +3220,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -3261,7 +3332,6 @@
       <c r="F5" s="3">
         <v>84</v>
       </c>
-      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
@@ -3352,7 +3422,7 @@
         <v>61</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -3374,7 +3444,6 @@
       <c r="F10" s="3">
         <v>48</v>
       </c>
-      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -3395,7 +3464,6 @@
       <c r="F11" s="3">
         <v>69</v>
       </c>
-      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -3416,9 +3484,11 @@
       <c r="F12" s="3">
         <v>79</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>45431</v>
       </c>
@@ -3437,12 +3507,12 @@
       <c r="F13" s="3">
         <v>58</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>13</v>
+      <c r="G13" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="8">
+      <c r="A14" s="2">
         <v>45436</v>
       </c>
       <c r="B14" s="3">
@@ -3461,6 +3531,29 @@
         <v>62</v>
       </c>
       <c r="G14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>45448</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1.35</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.63</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2.1</v>
+      </c>
+      <c r="E15" s="8">
+        <v>73</v>
+      </c>
+      <c r="F15" s="8">
+        <v>73</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>